<commit_message>
Google finance link added.
</commit_message>
<xml_diff>
--- a/stock.xlsx
+++ b/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFF4F4B-3037-45DB-B8AF-1F30E4B24E3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F15DDD6-52D5-45DF-AFA4-2F0FAF0A6798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>https://towardsdatascience.com/best-5-free-stock-market-apis-in-2019-ad91dddec984</t>
   </si>
   <si>
     <t>Best 5 free stock market APIs in 2020</t>
+  </si>
+  <si>
+    <t>https://support.google.com/docs/answer/3093281?hl=en</t>
+  </si>
+  <si>
+    <t>GOOGLE FINANCE</t>
   </si>
 </sst>
 </file>
@@ -348,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C2"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -368,6 +374,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>